<commit_message>
test Qt project created
</commit_message>
<xml_diff>
--- a/tests/TestDocument.xlsx
+++ b/tests/TestDocument.xlsx
@@ -24,8 +24,15 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts>
+	</numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>

</xml_diff>